<commit_message>
test double numbers are processed correctly
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheet_examples/test_spreadsheet_uncaptured.xlsx
+++ b/src/test/resources/spreadsheet_examples/test_spreadsheet_uncaptured.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/hard-data-hackathon-jvm/src/test/resources/spreadsheet_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/spreadsheet_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A33A752-DEAB-864F-AF39-0373022340EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0734191-8DF6-6444-8AB1-6DA36E8C2342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{870AAEF9-2DE1-494F-88CE-485EB3D1B417}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>string</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Alice</t>
+  </si>
+  <si>
+    <t>double</t>
   </si>
 </sst>
 </file>
@@ -429,18 +432,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B375211-7F82-3148-A5B5-8DEC9DA19438}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +460,11 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -473,8 +480,11 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2">
+        <v>1.05</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -487,8 +497,11 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -497,6 +510,9 @@
       </c>
       <c r="C4" s="3">
         <v>44199</v>
+      </c>
+      <c r="F4">
+        <v>3.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>